<commit_message>
Adjust preprocessing pipeline. Sort data by subject.
</commit_message>
<xml_diff>
--- a/raw-data-prep/raw_data/Debrief_HS.xlsx
+++ b/raw-data-prep/raw_data/Debrief_HS.xlsx
@@ -270,10 +270,10 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>GaMaybee.affect.distractioNo</t>
-  </si>
-  <si>
     <t>Maybe</t>
+  </si>
+  <si>
+    <t>Game.affect.distraction</t>
   </si>
 </sst>
 </file>
@@ -618,8 +618,8 @@
   <dimension ref="A1:R66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D53" sqref="D53"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,7 +671,7 @@
         <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="P1" t="s">
         <v>14</v>
@@ -1287,7 +1287,7 @@
         <v>0</v>
       </c>
       <c r="O12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P12" t="s">
         <v>82</v>
@@ -1343,7 +1343,7 @@
         <v>0</v>
       </c>
       <c r="O13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P13" t="s">
         <v>81</v>
@@ -1402,7 +1402,7 @@
         <v>81</v>
       </c>
       <c r="P14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q14">
         <v>1</v>
@@ -1455,7 +1455,7 @@
         <v>0</v>
       </c>
       <c r="O15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P15" t="s">
         <v>81</v>
@@ -1514,7 +1514,7 @@
         <v>81</v>
       </c>
       <c r="P16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q16">
         <v>4</v>
@@ -1567,7 +1567,7 @@
         <v>0</v>
       </c>
       <c r="O17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P17" t="s">
         <v>81</v>
@@ -1623,7 +1623,7 @@
         <v>0</v>
       </c>
       <c r="O18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P18" t="s">
         <v>82</v>
@@ -1903,7 +1903,7 @@
         <v>1</v>
       </c>
       <c r="O23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P23" t="s">
         <v>81</v>
@@ -2507,7 +2507,7 @@
         <v>0</v>
       </c>
       <c r="O34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P34" t="s">
         <v>82</v>
@@ -2566,7 +2566,7 @@
         <v>81</v>
       </c>
       <c r="P35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q35">
         <v>4</v>
@@ -2622,7 +2622,7 @@
         <v>81</v>
       </c>
       <c r="P36" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q36">
         <v>2</v>
@@ -2899,7 +2899,7 @@
         <v>0</v>
       </c>
       <c r="O41" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P41" t="s">
         <v>81</v>
@@ -2955,10 +2955,10 @@
         <v>0</v>
       </c>
       <c r="O42" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P42" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q42">
         <v>4</v>
@@ -3347,7 +3347,7 @@
         <v>0</v>
       </c>
       <c r="O49" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P49" t="s">
         <v>81</v>
@@ -3462,7 +3462,7 @@
         <v>81</v>
       </c>
       <c r="P51" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q51">
         <v>2</v>
@@ -3739,7 +3739,7 @@
         <v>1</v>
       </c>
       <c r="O56" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P56" t="s">
         <v>81</v>
@@ -4019,7 +4019,7 @@
         <v>0</v>
       </c>
       <c r="O61" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P61" t="s">
         <v>81</v>

</xml_diff>